<commit_message>
Add defender plan option
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0F5EFA-EF6C-4F04-9CE8-C1680883C79C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349D1B15-ACCB-42E5-B967-7F61EE235A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-160" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accelerator - Bootstrap" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1422" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="812">
   <si>
     <t>Description</t>
   </si>
@@ -2604,6 +2604,12 @@
   </si>
   <si>
     <t>Do you want to deploy AMBA policies?</t>
+  </si>
+  <si>
+    <t>Turn off Defender Plans</t>
+  </si>
+  <si>
+    <t>Do you want to turn off any defender plans?</t>
   </si>
 </sst>
 </file>
@@ -2896,7 +2902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3054,6 +3060,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -8546,7 +8555,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE440EAA-007A-486E-B4E3-7FE7599AA545}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -8746,7 +8755,7 @@
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="55" t="s">
         <v>790</v>
       </c>
       <c r="B14" s="39"/>
@@ -8977,13 +8986,30 @@
       <c r="F27" s="40"/>
       <c r="G27" s="34"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="36"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="43">
+        <v>13</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>810</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="D28" s="34"/>
+      <c r="E28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="40"/>
+      <c r="G28" s="34"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="36"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10277,6 +10303,58 @@
     <row r="116" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="E109:E110"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="C100:C101"/>
+    <mergeCell ref="E100:E101"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="E103:E104"/>
+    <mergeCell ref="A80:A94"/>
+    <mergeCell ref="B80:B94"/>
+    <mergeCell ref="C80:C94"/>
+    <mergeCell ref="E80:E94"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="E98:E99"/>
+    <mergeCell ref="A37:A64"/>
+    <mergeCell ref="B37:B64"/>
+    <mergeCell ref="C37:C64"/>
+    <mergeCell ref="E37:E64"/>
+    <mergeCell ref="A65:A79"/>
+    <mergeCell ref="B65:B79"/>
+    <mergeCell ref="C65:C79"/>
+    <mergeCell ref="E65:E79"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
@@ -10289,64 +10367,54 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="E10:E11"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A37:A64"/>
-    <mergeCell ref="B37:B64"/>
-    <mergeCell ref="C37:C64"/>
-    <mergeCell ref="E37:E64"/>
-    <mergeCell ref="A65:A79"/>
-    <mergeCell ref="B65:B79"/>
-    <mergeCell ref="C65:C79"/>
-    <mergeCell ref="E65:E79"/>
-    <mergeCell ref="A80:A94"/>
-    <mergeCell ref="B80:B94"/>
-    <mergeCell ref="C80:C94"/>
-    <mergeCell ref="E80:E94"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="E109:E110"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="B100:B101"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="E100:E101"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="E103:E104"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10688,49 +10756,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10751,33 +10804,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
fix: various minor fixes (#26)
* fix: various minor fixes

* Fix checklist typo

* Improve note

* Add warning about subscription placement

* fix typo
</commit_message>
<xml_diff>
--- a/docs/static/examples/tf/accelerator/config/checklist.xlsx
+++ b/docs/static/examples/tf/accelerator/config/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaredholgate\Code\azure-landing-zones\docs\static\examples\tf\accelerator\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349D1B15-ACCB-42E5-B967-7F61EE235A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5710D86-3326-4D36-8B2B-A43052A52008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="813">
   <si>
     <t>Description</t>
   </si>
@@ -2296,9 +2296,6 @@
     <t>a lower case string without spaces or punctuation</t>
   </si>
   <si>
-    <t>Resource naming: environemnt name</t>
-  </si>
-  <si>
     <t>The environment name segment of the default resource naming convention</t>
   </si>
   <si>
@@ -2610,6 +2607,12 @@
   </si>
   <si>
     <t>Do you want to turn off any defender plans?</t>
+  </si>
+  <si>
+    <t>Resource naming: environment name</t>
+  </si>
+  <si>
+    <t>"mgmt"</t>
   </si>
 </sst>
 </file>
@@ -3038,6 +3041,9 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3060,9 +3066,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3438,19 +3441,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="47" t="s">
-        <v>796</v>
-      </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="A1" s="48" t="s">
+        <v>795</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="44" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>672</v>
@@ -3523,7 +3526,7 @@
         <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F6" s="35"/>
       <c r="G6" s="34"/>
@@ -3703,7 +3706,9 @@
       <c r="E16" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="F16" s="35"/>
+      <c r="F16" s="35" t="s">
+        <v>16</v>
+      </c>
       <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -3711,10 +3716,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="34" t="s">
+        <v>811</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>709</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>710</v>
       </c>
       <c r="D17" s="34" t="s">
         <v>49</v>
@@ -3722,7 +3727,9 @@
       <c r="E17" s="1" t="s">
         <v>708</v>
       </c>
-      <c r="F17" s="35"/>
+      <c r="F17" s="35" t="s">
+        <v>812</v>
+      </c>
       <c r="G17" s="34"/>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -3730,18 +3737,20 @@
         <v>9</v>
       </c>
       <c r="B18" s="34" t="s">
+        <v>711</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>712</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>713</v>
       </c>
       <c r="D18" s="34" t="s">
         <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="F18" s="35"/>
+        <v>710</v>
+      </c>
+      <c r="F18" s="35">
+        <v>1</v>
+      </c>
       <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -3756,7 +3765,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="46"/>
       <c r="B20" s="39" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C20" s="37"/>
       <c r="D20" s="36"/>
@@ -3769,16 +3778,16 @@
         <v>11</v>
       </c>
       <c r="B21" s="34" t="s">
+        <v>727</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>728</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>729</v>
       </c>
       <c r="D21" s="34" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F21" s="40" t="s">
         <v>125</v>
@@ -3790,16 +3799,16 @@
         <v>10</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D22" s="34" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F22" s="40" t="s">
         <v>125</v>
@@ -3809,16 +3818,16 @@
     <row r="23" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="43"/>
       <c r="B23" s="34" t="s">
+        <v>732</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>733</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>734</v>
       </c>
       <c r="D23" s="34" t="s">
         <v>54</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F23" s="40" t="s">
         <v>141</v>
@@ -3830,20 +3839,20 @@
         <v>11</v>
       </c>
       <c r="B24" s="34" t="s">
+        <v>734</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>735</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>736</v>
       </c>
       <c r="D24" s="34" t="s">
         <v>55</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="34" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -3851,16 +3860,16 @@
         <v>11</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D25" s="34" t="s">
         <v>56</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F25" s="40" t="s">
         <v>125</v>
@@ -3879,7 +3888,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="46"/>
       <c r="B27" s="39" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C27" s="37"/>
       <c r="D27" s="36"/>
@@ -3892,10 +3901,10 @@
         <v>11</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D28" s="34" t="s">
         <v>57</v>
@@ -3909,10 +3918,10 @@
         <v>11</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="D29" s="34" t="s">
         <v>58</v>
@@ -3926,10 +3935,10 @@
         <v>11</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="D30" s="34" t="s">
         <v>59</v>
@@ -3943,16 +3952,16 @@
         <v>11</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="D31" s="34" t="s">
         <v>60</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F31" s="40" t="s">
         <v>141</v>
@@ -3964,16 +3973,16 @@
         <v>11</v>
       </c>
       <c r="B32" s="34" t="s">
+        <v>748</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>749</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>750</v>
       </c>
       <c r="D32" s="34" t="s">
         <v>61</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F32" s="40" t="s">
         <v>125</v>
@@ -3985,10 +3994,10 @@
         <v>11</v>
       </c>
       <c r="B33" s="34" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D33" s="34" t="s">
         <v>62</v>
@@ -4002,10 +4011,10 @@
         <v>10</v>
       </c>
       <c r="B34" s="34" t="s">
+        <v>751</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>752</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>753</v>
       </c>
       <c r="D34" s="34" t="s">
         <v>52</v>
@@ -4028,7 +4037,7 @@
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="46"/>
       <c r="B36" s="39" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C36" s="37"/>
       <c r="D36" s="36"/>
@@ -4041,10 +4050,10 @@
         <v>11</v>
       </c>
       <c r="B37" s="34" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D37" s="34" t="s">
         <v>63</v>
@@ -4058,10 +4067,10 @@
         <v>11</v>
       </c>
       <c r="B38" s="34" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D38" s="34" t="s">
         <v>64</v>
@@ -4075,10 +4084,10 @@
         <v>11</v>
       </c>
       <c r="B39" s="34" t="s">
+        <v>755</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>756</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>757</v>
       </c>
       <c r="D39" s="34" t="s">
         <v>65</v>
@@ -4092,10 +4101,10 @@
         <v>10</v>
       </c>
       <c r="B40" s="34" t="s">
+        <v>753</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>754</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>755</v>
       </c>
       <c r="D40" s="34" t="s">
         <v>514</v>
@@ -4118,7 +4127,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="46"/>
       <c r="B42" s="39" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C42" s="37"/>
       <c r="D42" s="36"/>
@@ -4131,16 +4140,16 @@
         <v>11</v>
       </c>
       <c r="B43" s="34" t="s">
+        <v>714</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>715</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>716</v>
       </c>
       <c r="D43" s="34" t="s">
         <v>66</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F43" s="40" t="s">
         <v>44</v>
@@ -4152,16 +4161,16 @@
         <v>11</v>
       </c>
       <c r="B44" s="34" t="s">
+        <v>717</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>718</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="D44" s="34" t="s">
+        <v>720</v>
+      </c>
+      <c r="E44" s="1" t="s">
         <v>719</v>
-      </c>
-      <c r="D44" s="34" t="s">
-        <v>721</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>720</v>
       </c>
       <c r="F44" s="40" t="s">
         <v>125</v>
@@ -4173,16 +4182,16 @@
         <v>11</v>
       </c>
       <c r="B45" s="34" t="s">
+        <v>721</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D45" s="34" t="s">
         <v>722</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="D45" s="34" t="s">
-        <v>723</v>
-      </c>
       <c r="E45" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F45" s="40" t="s">
         <v>125</v>
@@ -8573,19 +8582,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="77.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
-        <v>797</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
+      <c r="A1" s="49" t="s">
+        <v>796</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="41" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>672</v>
@@ -8617,7 +8626,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="39" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="37"/>
@@ -8631,10 +8640,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="1" t="s">
@@ -8648,10 +8657,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="1" t="s">
@@ -8665,10 +8674,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="34" t="s">
+        <v>765</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>766</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>767</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="1" t="s">
@@ -8682,10 +8691,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="34" t="s">
+        <v>767</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>768</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>769</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="1" t="s">
@@ -8699,10 +8708,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="34" t="s">
+        <v>773</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>774</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>775</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="1" t="s">
@@ -8716,10 +8725,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="34" t="s">
+        <v>769</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>770</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>771</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="1" t="s">
@@ -8733,10 +8742,10 @@
         <v>7</v>
       </c>
       <c r="B12" s="34" t="s">
+        <v>771</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>772</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>773</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="1" t="s">
@@ -8755,8 +8764,8 @@
       <c r="G13" s="36"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="55" t="s">
-        <v>790</v>
+      <c r="A14" s="47" t="s">
+        <v>789</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="37"/>
@@ -8770,14 +8779,14 @@
         <v>1</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="34"/>
@@ -8787,10 +8796,10 @@
         <v>2</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="1" t="s">
@@ -8804,10 +8813,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="1" t="s">
@@ -8821,10 +8830,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="1" t="s">
@@ -8838,10 +8847,10 @@
         <v>5</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="1" t="s">
@@ -8858,7 +8867,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="1" t="s">
@@ -8875,7 +8884,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="1" t="s">
@@ -8889,10 +8898,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="34" t="s">
+        <v>790</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>792</v>
       </c>
       <c r="D22" s="34"/>
       <c r="E22" s="1" t="s">
@@ -8906,14 +8915,14 @@
         <v>8</v>
       </c>
       <c r="B23" s="34" t="s">
+        <v>792</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>793</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>794</v>
       </c>
       <c r="D23" s="34"/>
       <c r="E23" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F23" s="40"/>
       <c r="G23" s="34"/>
@@ -8923,14 +8932,14 @@
         <v>9</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F24" s="35"/>
       <c r="G24" s="34"/>
@@ -8940,14 +8949,14 @@
         <v>10</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="D25" s="34"/>
       <c r="E25" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F25" s="40"/>
       <c r="G25" s="34"/>
@@ -8957,10 +8966,10 @@
         <v>11</v>
       </c>
       <c r="B26" s="34" t="s">
+        <v>800</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>801</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>802</v>
       </c>
       <c r="D26" s="34"/>
       <c r="E26" s="1" t="s">
@@ -8974,10 +8983,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="34" t="s">
+        <v>807</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>808</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>809</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="1" t="s">
@@ -8991,10 +9000,10 @@
         <v>13</v>
       </c>
       <c r="B28" s="34" t="s">
+        <v>809</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>810</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>811</v>
       </c>
       <c r="D28" s="34"/>
       <c r="E28" s="1" t="s">
@@ -9119,39 +9128,39 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="52" t="s">
+      <c r="A6" s="53" t="s">
         <v>515</v>
       </c>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="54" t="s">
         <v>531</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="54" t="s">
         <v>532</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>533</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="55" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
+      <c r="A7" s="53"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="17" t="s">
         <v>534</v>
       </c>
-      <c r="E7" s="54"/>
+      <c r="E7" s="55"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
+      <c r="A8" s="53"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="17" t="s">
         <v>535</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="55"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="19" t="s">
@@ -9171,56 +9180,56 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="53" t="s">
         <v>515</v>
       </c>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="54" t="s">
         <v>540</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="54" t="s">
         <v>541</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>542</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="55" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="52"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="54"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="17" t="s">
         <v>544</v>
       </c>
-      <c r="E11" s="54"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="50" t="s">
         <v>515</v>
       </c>
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="51" t="s">
         <v>545</v>
       </c>
-      <c r="C12" s="50" t="s">
+      <c r="C12" s="51" t="s">
         <v>546</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>547</v>
       </c>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="52" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="49"/>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
       <c r="D13" s="20" t="s">
         <v>549</v>
       </c>
-      <c r="E13" s="51"/>
+      <c r="E13" s="52"/>
     </row>
     <row r="14" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
@@ -9375,148 +9384,148 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="52"/>
-      <c r="B24" s="53" t="s">
+      <c r="A24" s="53"/>
+      <c r="B24" s="54" t="s">
         <v>573</v>
       </c>
-      <c r="C24" s="53" t="s">
+      <c r="C24" s="54" t="s">
         <v>574</v>
       </c>
       <c r="D24" s="17" t="s">
         <v>575</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="55" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="52"/>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
+      <c r="A25" s="53"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
       <c r="D25" s="17" t="s">
         <v>577</v>
       </c>
-      <c r="E25" s="54"/>
+      <c r="E25" s="55"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="49"/>
-      <c r="B26" s="50" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="51" t="s">
         <v>578</v>
       </c>
-      <c r="C26" s="50" t="s">
+      <c r="C26" s="51" t="s">
         <v>579</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>580</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="52" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="49"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="20" t="s">
         <v>582</v>
       </c>
-      <c r="E27" s="51"/>
+      <c r="E27" s="52"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="52"/>
-      <c r="B28" s="53" t="s">
+      <c r="A28" s="53"/>
+      <c r="B28" s="54" t="s">
         <v>583</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C28" s="54" t="s">
         <v>584</v>
       </c>
       <c r="D28" s="17" t="s">
         <v>580</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="55" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="52"/>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="54"/>
       <c r="D29" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="E29" s="54"/>
+      <c r="E29" s="55"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="49"/>
-      <c r="B30" s="50" t="s">
+      <c r="A30" s="50"/>
+      <c r="B30" s="51" t="s">
         <v>587</v>
       </c>
-      <c r="C30" s="50" t="s">
+      <c r="C30" s="51" t="s">
         <v>588</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>580</v>
       </c>
-      <c r="E30" s="51" t="s">
+      <c r="E30" s="52" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="49"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
       <c r="D31" s="20" t="s">
         <v>589</v>
       </c>
-      <c r="E31" s="51"/>
+      <c r="E31" s="52"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="52"/>
-      <c r="B32" s="53" t="s">
+      <c r="A32" s="53"/>
+      <c r="B32" s="54" t="s">
         <v>590</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="C32" s="54" t="s">
         <v>591</v>
       </c>
       <c r="D32" s="17" t="s">
         <v>592</v>
       </c>
-      <c r="E32" s="54" t="s">
+      <c r="E32" s="55" t="s">
         <v>593</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="52"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="54"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="17" t="s">
         <v>594</v>
       </c>
-      <c r="E33" s="54"/>
+      <c r="E33" s="55"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="49"/>
-      <c r="B34" s="50" t="s">
+      <c r="A34" s="50"/>
+      <c r="B34" s="51" t="s">
         <v>595</v>
       </c>
-      <c r="C34" s="50" t="s">
+      <c r="C34" s="51" t="s">
         <v>596</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>597</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="52" t="s">
         <v>598</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="49"/>
-      <c r="B35" s="50"/>
-      <c r="C35" s="50"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="51"/>
+      <c r="C35" s="51"/>
       <c r="D35" s="20" t="s">
         <v>599</v>
       </c>
-      <c r="E35" s="51"/>
+      <c r="E35" s="52"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="16"/>
@@ -9534,536 +9543,536 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="49"/>
-      <c r="B37" s="50" t="s">
+      <c r="A37" s="50"/>
+      <c r="B37" s="51" t="s">
         <v>602</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="51" t="s">
         <v>603</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E37" s="52" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="49"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="51"/>
       <c r="D38" s="20" t="s">
         <v>606</v>
       </c>
-      <c r="E38" s="51"/>
+      <c r="E38" s="52"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="49"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="50"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
       <c r="D39" s="20" t="s">
         <v>607</v>
       </c>
-      <c r="E39" s="51"/>
+      <c r="E39" s="52"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="49"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="50"/>
+      <c r="A40" s="50"/>
+      <c r="B40" s="51"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="20" t="s">
         <v>608</v>
       </c>
-      <c r="E40" s="51"/>
+      <c r="E40" s="52"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="49"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
+      <c r="A41" s="50"/>
+      <c r="B41" s="51"/>
+      <c r="C41" s="51"/>
       <c r="D41" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="E41" s="51"/>
+      <c r="E41" s="52"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="49"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
+      <c r="A42" s="50"/>
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
       <c r="D42" s="20" t="s">
         <v>610</v>
       </c>
-      <c r="E42" s="51"/>
+      <c r="E42" s="52"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="49"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
       <c r="D43" s="20" t="s">
         <v>611</v>
       </c>
-      <c r="E43" s="51"/>
+      <c r="E43" s="52"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="49"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
+      <c r="A44" s="50"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
       <c r="D44" s="20" t="s">
         <v>612</v>
       </c>
-      <c r="E44" s="51"/>
+      <c r="E44" s="52"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="49"/>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
+      <c r="A45" s="50"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
       <c r="D45" s="20" t="s">
         <v>613</v>
       </c>
-      <c r="E45" s="51"/>
+      <c r="E45" s="52"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="49"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50"/>
+      <c r="A46" s="50"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
       <c r="D46" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="E46" s="51"/>
+      <c r="E46" s="52"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="49"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="50"/>
+      <c r="A47" s="50"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="51"/>
+      <c r="E47" s="52"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="49"/>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
+      <c r="A48" s="50"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
       <c r="D48" s="20" t="s">
         <v>606</v>
       </c>
-      <c r="E48" s="51"/>
+      <c r="E48" s="52"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="49"/>
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
+      <c r="A49" s="50"/>
+      <c r="B49" s="51"/>
+      <c r="C49" s="51"/>
       <c r="D49" s="20" t="s">
         <v>607</v>
       </c>
-      <c r="E49" s="51"/>
+      <c r="E49" s="52"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="49"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
+      <c r="A50" s="50"/>
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
       <c r="D50" s="20" t="s">
         <v>608</v>
       </c>
-      <c r="E50" s="51"/>
+      <c r="E50" s="52"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="49"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="50"/>
+      <c r="A51" s="50"/>
+      <c r="B51" s="51"/>
+      <c r="C51" s="51"/>
       <c r="D51" s="20" t="s">
         <v>609</v>
       </c>
-      <c r="E51" s="51"/>
+      <c r="E51" s="52"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="49"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="50"/>
+      <c r="A52" s="50"/>
+      <c r="B52" s="51"/>
+      <c r="C52" s="51"/>
       <c r="D52" s="20" t="s">
         <v>610</v>
       </c>
-      <c r="E52" s="51"/>
+      <c r="E52" s="52"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="49"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="50"/>
+      <c r="A53" s="50"/>
+      <c r="B53" s="51"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="20" t="s">
         <v>611</v>
       </c>
-      <c r="E53" s="51"/>
+      <c r="E53" s="52"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="49"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="50"/>
+      <c r="A54" s="50"/>
+      <c r="B54" s="51"/>
+      <c r="C54" s="51"/>
       <c r="D54" s="20" t="s">
         <v>612</v>
       </c>
-      <c r="E54" s="51"/>
+      <c r="E54" s="52"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="49"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="50"/>
+      <c r="A55" s="50"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
       <c r="D55" s="20" t="s">
         <v>613</v>
       </c>
-      <c r="E55" s="51"/>
+      <c r="E55" s="52"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="49"/>
-      <c r="B56" s="50"/>
-      <c r="C56" s="50"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="51"/>
       <c r="D56" s="20" t="s">
         <v>614</v>
       </c>
-      <c r="E56" s="51"/>
+      <c r="E56" s="52"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="49"/>
-      <c r="B57" s="50"/>
-      <c r="C57" s="50"/>
+      <c r="A57" s="50"/>
+      <c r="B57" s="51"/>
+      <c r="C57" s="51"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="51"/>
+      <c r="E57" s="52"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="49"/>
-      <c r="B58" s="50"/>
-      <c r="C58" s="50"/>
+      <c r="A58" s="50"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="51"/>
       <c r="D58" s="20" t="s">
         <v>615</v>
       </c>
-      <c r="E58" s="51"/>
+      <c r="E58" s="52"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="49"/>
-      <c r="B59" s="50"/>
-      <c r="C59" s="50"/>
+      <c r="A59" s="50"/>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
       <c r="D59" s="20" t="s">
         <v>616</v>
       </c>
-      <c r="E59" s="51"/>
+      <c r="E59" s="52"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="49"/>
-      <c r="B60" s="50"/>
-      <c r="C60" s="50"/>
+      <c r="A60" s="50"/>
+      <c r="B60" s="51"/>
+      <c r="C60" s="51"/>
       <c r="D60" s="20" t="s">
         <v>617</v>
       </c>
-      <c r="E60" s="51"/>
+      <c r="E60" s="52"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="49"/>
-      <c r="B61" s="50"/>
-      <c r="C61" s="50"/>
+      <c r="A61" s="50"/>
+      <c r="B61" s="51"/>
+      <c r="C61" s="51"/>
       <c r="D61" s="20" t="s">
         <v>618</v>
       </c>
-      <c r="E61" s="51"/>
+      <c r="E61" s="52"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="49"/>
-      <c r="B62" s="50"/>
-      <c r="C62" s="50"/>
+      <c r="A62" s="50"/>
+      <c r="B62" s="51"/>
+      <c r="C62" s="51"/>
       <c r="D62" s="20" t="s">
         <v>619</v>
       </c>
-      <c r="E62" s="51"/>
+      <c r="E62" s="52"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="49"/>
-      <c r="B63" s="50"/>
-      <c r="C63" s="50"/>
+      <c r="A63" s="50"/>
+      <c r="B63" s="51"/>
+      <c r="C63" s="51"/>
       <c r="D63" s="20" t="s">
         <v>620</v>
       </c>
-      <c r="E63" s="51"/>
+      <c r="E63" s="52"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="49"/>
-      <c r="B64" s="50"/>
-      <c r="C64" s="50"/>
+      <c r="A64" s="50"/>
+      <c r="B64" s="51"/>
+      <c r="C64" s="51"/>
       <c r="D64" s="20" t="s">
         <v>621</v>
       </c>
-      <c r="E64" s="51"/>
+      <c r="E64" s="52"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="52"/>
-      <c r="B65" s="53" t="s">
+      <c r="A65" s="53"/>
+      <c r="B65" s="54" t="s">
         <v>248</v>
       </c>
-      <c r="C65" s="53" t="s">
+      <c r="C65" s="54" t="s">
         <v>622</v>
       </c>
       <c r="D65" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="E65" s="54" t="s">
+      <c r="E65" s="55" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="52"/>
-      <c r="B66" s="53"/>
-      <c r="C66" s="53"/>
+      <c r="A66" s="53"/>
+      <c r="B66" s="54"/>
+      <c r="C66" s="54"/>
       <c r="D66" s="22"/>
-      <c r="E66" s="54"/>
+      <c r="E66" s="55"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="52"/>
-      <c r="B67" s="53"/>
-      <c r="C67" s="53"/>
+      <c r="A67" s="53"/>
+      <c r="B67" s="54"/>
+      <c r="C67" s="54"/>
       <c r="D67" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="E67" s="54"/>
+      <c r="E67" s="55"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="52"/>
-      <c r="B68" s="53"/>
-      <c r="C68" s="53"/>
+      <c r="A68" s="53"/>
+      <c r="B68" s="54"/>
+      <c r="C68" s="54"/>
       <c r="D68" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="E68" s="54"/>
+      <c r="E68" s="55"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="52"/>
-      <c r="B69" s="53"/>
-      <c r="C69" s="53"/>
+      <c r="A69" s="53"/>
+      <c r="B69" s="54"/>
+      <c r="C69" s="54"/>
       <c r="D69" s="17" t="s">
         <v>625</v>
       </c>
-      <c r="E69" s="54"/>
+      <c r="E69" s="55"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="52"/>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
+      <c r="A70" s="53"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
       <c r="D70" s="17" t="s">
         <v>626</v>
       </c>
-      <c r="E70" s="54"/>
+      <c r="E70" s="55"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="52"/>
-      <c r="B71" s="53"/>
-      <c r="C71" s="53"/>
+      <c r="A71" s="53"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
       <c r="D71" s="17" t="s">
         <v>627</v>
       </c>
-      <c r="E71" s="54"/>
+      <c r="E71" s="55"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="52"/>
-      <c r="B72" s="53"/>
-      <c r="C72" s="53"/>
+      <c r="A72" s="53"/>
+      <c r="B72" s="54"/>
+      <c r="C72" s="54"/>
       <c r="D72" s="17" t="s">
         <v>628</v>
       </c>
-      <c r="E72" s="54"/>
+      <c r="E72" s="55"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="52"/>
-      <c r="B73" s="53"/>
-      <c r="C73" s="53"/>
+      <c r="A73" s="53"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="54"/>
       <c r="D73" s="17" t="s">
         <v>629</v>
       </c>
-      <c r="E73" s="54"/>
+      <c r="E73" s="55"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="52"/>
-      <c r="B74" s="53"/>
-      <c r="C74" s="53"/>
+      <c r="A74" s="53"/>
+      <c r="B74" s="54"/>
+      <c r="C74" s="54"/>
       <c r="D74" s="17" t="s">
         <v>630</v>
       </c>
-      <c r="E74" s="54"/>
+      <c r="E74" s="55"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="52"/>
-      <c r="B75" s="53"/>
-      <c r="C75" s="53"/>
+      <c r="A75" s="53"/>
+      <c r="B75" s="54"/>
+      <c r="C75" s="54"/>
       <c r="D75" s="17" t="s">
         <v>631</v>
       </c>
-      <c r="E75" s="54"/>
+      <c r="E75" s="55"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" s="52"/>
-      <c r="B76" s="53"/>
-      <c r="C76" s="53"/>
+      <c r="A76" s="53"/>
+      <c r="B76" s="54"/>
+      <c r="C76" s="54"/>
       <c r="D76" s="17" t="s">
         <v>632</v>
       </c>
-      <c r="E76" s="54"/>
+      <c r="E76" s="55"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="52"/>
-      <c r="B77" s="53"/>
-      <c r="C77" s="53"/>
+      <c r="A77" s="53"/>
+      <c r="B77" s="54"/>
+      <c r="C77" s="54"/>
       <c r="D77" s="17" t="s">
         <v>633</v>
       </c>
-      <c r="E77" s="54"/>
+      <c r="E77" s="55"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" s="52"/>
-      <c r="B78" s="53"/>
-      <c r="C78" s="53"/>
+      <c r="A78" s="53"/>
+      <c r="B78" s="54"/>
+      <c r="C78" s="54"/>
       <c r="D78" s="17" t="s">
         <v>634</v>
       </c>
-      <c r="E78" s="54"/>
+      <c r="E78" s="55"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" s="52"/>
-      <c r="B79" s="53"/>
-      <c r="C79" s="53"/>
+      <c r="A79" s="53"/>
+      <c r="B79" s="54"/>
+      <c r="C79" s="54"/>
       <c r="D79" s="17" t="s">
         <v>635</v>
       </c>
-      <c r="E79" s="54"/>
+      <c r="E79" s="55"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" s="49"/>
-      <c r="B80" s="50" t="s">
+      <c r="A80" s="50"/>
+      <c r="B80" s="51" t="s">
         <v>245</v>
       </c>
-      <c r="C80" s="50" t="s">
+      <c r="C80" s="51" t="s">
         <v>636</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>637</v>
       </c>
-      <c r="E80" s="51" t="s">
+      <c r="E80" s="52" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" s="49"/>
-      <c r="B81" s="50"/>
-      <c r="C81" s="50"/>
+      <c r="A81" s="50"/>
+      <c r="B81" s="51"/>
+      <c r="C81" s="51"/>
       <c r="D81" s="3"/>
-      <c r="E81" s="51"/>
+      <c r="E81" s="52"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" s="49"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
+      <c r="A82" s="50"/>
+      <c r="B82" s="51"/>
+      <c r="C82" s="51"/>
       <c r="D82" s="20" t="s">
         <v>604</v>
       </c>
-      <c r="E82" s="51"/>
+      <c r="E82" s="52"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" s="49"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="50"/>
+      <c r="A83" s="50"/>
+      <c r="B83" s="51"/>
+      <c r="C83" s="51"/>
       <c r="D83" s="20" t="s">
         <v>624</v>
       </c>
-      <c r="E83" s="51"/>
+      <c r="E83" s="52"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" s="49"/>
-      <c r="B84" s="50"/>
-      <c r="C84" s="50"/>
+      <c r="A84" s="50"/>
+      <c r="B84" s="51"/>
+      <c r="C84" s="51"/>
       <c r="D84" s="20" t="s">
         <v>638</v>
       </c>
-      <c r="E84" s="51"/>
+      <c r="E84" s="52"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" s="49"/>
-      <c r="B85" s="50"/>
-      <c r="C85" s="50"/>
+      <c r="A85" s="50"/>
+      <c r="B85" s="51"/>
+      <c r="C85" s="51"/>
       <c r="D85" s="20" t="s">
         <v>626</v>
       </c>
-      <c r="E85" s="51"/>
+      <c r="E85" s="52"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" s="49"/>
-      <c r="B86" s="50"/>
-      <c r="C86" s="50"/>
+      <c r="A86" s="50"/>
+      <c r="B86" s="51"/>
+      <c r="C86" s="51"/>
       <c r="D86" s="20" t="s">
         <v>639</v>
       </c>
-      <c r="E86" s="51"/>
+      <c r="E86" s="52"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" s="49"/>
-      <c r="B87" s="50"/>
-      <c r="C87" s="50"/>
+      <c r="A87" s="50"/>
+      <c r="B87" s="51"/>
+      <c r="C87" s="51"/>
       <c r="D87" s="20" t="s">
         <v>628</v>
       </c>
-      <c r="E87" s="51"/>
+      <c r="E87" s="52"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" s="49"/>
-      <c r="B88" s="50"/>
-      <c r="C88" s="50"/>
+      <c r="A88" s="50"/>
+      <c r="B88" s="51"/>
+      <c r="C88" s="51"/>
       <c r="D88" s="20" t="s">
         <v>629</v>
       </c>
-      <c r="E88" s="51"/>
+      <c r="E88" s="52"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" s="49"/>
-      <c r="B89" s="50"/>
-      <c r="C89" s="50"/>
+      <c r="A89" s="50"/>
+      <c r="B89" s="51"/>
+      <c r="C89" s="51"/>
       <c r="D89" s="20" t="s">
         <v>630</v>
       </c>
-      <c r="E89" s="51"/>
+      <c r="E89" s="52"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" s="49"/>
-      <c r="B90" s="50"/>
-      <c r="C90" s="50"/>
+      <c r="A90" s="50"/>
+      <c r="B90" s="51"/>
+      <c r="C90" s="51"/>
       <c r="D90" s="20" t="s">
         <v>631</v>
       </c>
-      <c r="E90" s="51"/>
+      <c r="E90" s="52"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" s="49"/>
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
+      <c r="A91" s="50"/>
+      <c r="B91" s="51"/>
+      <c r="C91" s="51"/>
       <c r="D91" s="20" t="s">
         <v>632</v>
       </c>
-      <c r="E91" s="51"/>
+      <c r="E91" s="52"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" s="49"/>
-      <c r="B92" s="50"/>
-      <c r="C92" s="50"/>
+      <c r="A92" s="50"/>
+      <c r="B92" s="51"/>
+      <c r="C92" s="51"/>
       <c r="D92" s="20" t="s">
         <v>633</v>
       </c>
-      <c r="E92" s="51"/>
+      <c r="E92" s="52"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" s="49"/>
-      <c r="B93" s="50"/>
-      <c r="C93" s="50"/>
+      <c r="A93" s="50"/>
+      <c r="B93" s="51"/>
+      <c r="C93" s="51"/>
       <c r="D93" s="20" t="s">
         <v>634</v>
       </c>
-      <c r="E93" s="51"/>
+      <c r="E93" s="52"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A94" s="49"/>
-      <c r="B94" s="50"/>
-      <c r="C94" s="50"/>
+      <c r="A94" s="50"/>
+      <c r="B94" s="51"/>
+      <c r="C94" s="51"/>
       <c r="D94" s="20" t="s">
         <v>635</v>
       </c>
-      <c r="E94" s="51"/>
+      <c r="E94" s="52"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="16"/>
@@ -10111,52 +10120,52 @@
       </c>
     </row>
     <row r="98" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A98" s="49"/>
-      <c r="B98" s="50" t="s">
+      <c r="A98" s="50"/>
+      <c r="B98" s="51" t="s">
         <v>126</v>
       </c>
-      <c r="C98" s="50" t="s">
+      <c r="C98" s="51" t="s">
         <v>646</v>
       </c>
       <c r="D98" s="20" t="s">
         <v>647</v>
       </c>
-      <c r="E98" s="51" t="s">
+      <c r="E98" s="52" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A99" s="49"/>
-      <c r="B99" s="50"/>
-      <c r="C99" s="50"/>
+      <c r="A99" s="50"/>
+      <c r="B99" s="51"/>
+      <c r="C99" s="51"/>
       <c r="D99" s="20" t="s">
         <v>648</v>
       </c>
-      <c r="E99" s="51"/>
+      <c r="E99" s="52"/>
     </row>
     <row r="100" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="52"/>
-      <c r="B100" s="53" t="s">
+      <c r="A100" s="53"/>
+      <c r="B100" s="54" t="s">
         <v>499</v>
       </c>
-      <c r="C100" s="53" t="s">
+      <c r="C100" s="54" t="s">
         <v>649</v>
       </c>
       <c r="D100" s="17" t="s">
         <v>650</v>
       </c>
-      <c r="E100" s="54" t="s">
+      <c r="E100" s="55" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A101" s="52"/>
-      <c r="B101" s="53"/>
-      <c r="C101" s="53"/>
+      <c r="A101" s="53"/>
+      <c r="B101" s="54"/>
+      <c r="C101" s="54"/>
       <c r="D101" s="17" t="s">
         <v>651</v>
       </c>
-      <c r="E101" s="54"/>
+      <c r="E101" s="55"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="19"/>
@@ -10174,28 +10183,28 @@
       </c>
     </row>
     <row r="103" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="52"/>
-      <c r="B103" s="53" t="s">
+      <c r="A103" s="53"/>
+      <c r="B103" s="54" t="s">
         <v>653</v>
       </c>
-      <c r="C103" s="53" t="s">
+      <c r="C103" s="54" t="s">
         <v>654</v>
       </c>
       <c r="D103" s="17" t="s">
         <v>655</v>
       </c>
-      <c r="E103" s="54" t="s">
+      <c r="E103" s="55" t="s">
         <v>555</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A104" s="52"/>
-      <c r="B104" s="53"/>
-      <c r="C104" s="53"/>
+      <c r="A104" s="53"/>
+      <c r="B104" s="54"/>
+      <c r="C104" s="54"/>
       <c r="D104" s="17" t="s">
         <v>656</v>
       </c>
-      <c r="E104" s="54"/>
+      <c r="E104" s="55"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="19"/>
@@ -10258,28 +10267,28 @@
       </c>
     </row>
     <row r="109" spans="1:5" ht="12.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A109" s="49"/>
-      <c r="B109" s="50" t="s">
+      <c r="A109" s="50"/>
+      <c r="B109" s="51" t="s">
         <v>666</v>
       </c>
-      <c r="C109" s="50" t="s">
+      <c r="C109" s="51" t="s">
         <v>667</v>
       </c>
       <c r="D109" s="20" t="s">
         <v>668</v>
       </c>
-      <c r="E109" s="51" t="s">
+      <c r="E109" s="52" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A110" s="49"/>
-      <c r="B110" s="50"/>
-      <c r="C110" s="50"/>
+      <c r="A110" s="50"/>
+      <c r="B110" s="51"/>
+      <c r="C110" s="51"/>
       <c r="D110" s="20" t="s">
         <v>669</v>
       </c>
-      <c r="E110" s="51"/>
+      <c r="E110" s="52"/>
     </row>
     <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="23"/>
@@ -10303,6 +10312,58 @@
     <row r="116" hidden="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="A37:A64"/>
+    <mergeCell ref="B37:B64"/>
+    <mergeCell ref="C37:C64"/>
+    <mergeCell ref="E37:E64"/>
+    <mergeCell ref="A65:A79"/>
+    <mergeCell ref="B65:B79"/>
+    <mergeCell ref="C65:C79"/>
+    <mergeCell ref="E65:E79"/>
+    <mergeCell ref="A80:A94"/>
+    <mergeCell ref="B80:B94"/>
+    <mergeCell ref="C80:C94"/>
+    <mergeCell ref="E80:E94"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="B98:B99"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="E98:E99"/>
     <mergeCell ref="A109:A110"/>
     <mergeCell ref="B109:B110"/>
     <mergeCell ref="C109:C110"/>
@@ -10315,106 +10376,12 @@
     <mergeCell ref="B103:B104"/>
     <mergeCell ref="C103:C104"/>
     <mergeCell ref="E103:E104"/>
-    <mergeCell ref="A80:A94"/>
-    <mergeCell ref="B80:B94"/>
-    <mergeCell ref="C80:C94"/>
-    <mergeCell ref="E80:E94"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="E98:E99"/>
-    <mergeCell ref="A37:A64"/>
-    <mergeCell ref="B37:B64"/>
-    <mergeCell ref="C37:C64"/>
-    <mergeCell ref="E37:E64"/>
-    <mergeCell ref="A65:A79"/>
-    <mergeCell ref="B65:B79"/>
-    <mergeCell ref="C65:C79"/>
-    <mergeCell ref="E65:E79"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Title_x0020_URL>
-    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
-    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
-    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
-    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010039A62E282DDA434E979CD3E03185182E" ma:contentTypeVersion="33" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6c69cf93bfe1fca5d0e373365e7fdfc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="cea7764e-6bf9-427d-be15-e74097e0a61c" xmlns:ns3="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62cb4c6faf5eab163d0c8ea23c8ff408" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -10756,34 +10723,49 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <MediaLengthInSeconds xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Sign_x002d_off_x0020_status xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Title_x0020_URL xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Title_x0020_URL>
+    <Mail_x0020_Sent xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Mail_x0020_Sent>
+    <_Flow_SignoffStatus xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <State xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">Open</State>
+    <Comments xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <Lead_x0020_Signoff xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c">false</Lead_x0020_Signoff>
+    <Title_x0020_ID xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+    <TranslatedLang xmlns="cea7764e-6bf9-427d-be15-e74097e0a61c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23B9621B-458A-4676-8042-F53348150B3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10804,6 +10786,33 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F377113-5718-41B1-A1CE-B96F830D3573}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E53D8182-34C2-4EE5-8FD0-D750C3EB0900}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="fb9ea31f-0ab8-44ff-80d1-5777f6d9d945"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="cea7764e-6bf9-427d-be15-e74097e0a61c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{87867195-f2b8-4ac2-b0b6-6bb73cb33afc}" enabled="1" method="Privileged" siteId="{72f988bf-86f1-41af-91ab-2d7cd011db47}" contentBits="0" removed="0"/>

</xml_diff>